<commit_message>
update for 4 week
</commit_message>
<xml_diff>
--- a/0_docs/CheckListForm_3week.xlsx
+++ b/0_docs/CheckListForm_3week.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\유도진\Dropbox\MJU\Coin\2.study\21_1\Study-21-1-codingTest\0_docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DOJINYOU\Dropbox\MJU\Coin\2.study\21_1\Study-21-1-codingTest\0_docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA52290B-3956-406F-A8B1-277C282BA4B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22138403-6FC6-41E7-B663-1FE5D7D347C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="645" windowWidth="14355" windowHeight="15555" xr2:uid="{2683A084-5E1C-45DB-8DAE-141C5F5642CD}"/>
+    <workbookView xWindow="3588" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{2683A084-5E1C-45DB-8DAE-141C5F5642CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="51">
   <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -234,14 +234,6 @@
   </si>
   <si>
     <t>https://www.acmicpc.net/problem/7490</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>중량제한</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://www.acmicpc.net/problem/1939</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -788,14 +780,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1114,27 +1106,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA290B9-D938-4FB9-A2F0-C9496544FB19}">
   <dimension ref="B1:V194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="3.25" customWidth="1"/>
-    <col min="2" max="2" width="9.75" customWidth="1"/>
-    <col min="3" max="3" width="4.625" customWidth="1"/>
-    <col min="4" max="4" width="39.125" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="16.875" customWidth="1"/>
+    <col min="1" max="1" width="3.19921875" customWidth="1"/>
+    <col min="2" max="2" width="9.69921875" customWidth="1"/>
+    <col min="3" max="3" width="4.59765625" customWidth="1"/>
+    <col min="4" max="4" width="39.09765625" customWidth="1"/>
+    <col min="5" max="5" width="14.3984375" customWidth="1"/>
+    <col min="6" max="6" width="16.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="31" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="32"/>
-      <c r="D2" s="37"/>
+      <c r="D2" s="35"/>
       <c r="E2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1142,14 +1134,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:6" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:6" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B4" s="27" t="s">
         <v>3</v>
       </c>
@@ -1162,7 +1154,7 @@
       </c>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B5" s="29" t="s">
         <v>2</v>
       </c>
@@ -1177,7 +1169,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B6" s="31" t="s">
         <v>5</v>
       </c>
@@ -1186,7 +1178,7 @@
       <c r="E6" s="32"/>
       <c r="F6" s="33"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B7" s="34" t="s">
         <v>17</v>
       </c>
@@ -1197,7 +1189,7 @@
       <c r="E7" s="19"/>
       <c r="F7" s="20"/>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B8" s="16"/>
       <c r="C8" s="4"/>
       <c r="D8" s="21" t="s">
@@ -1206,7 +1198,7 @@
       <c r="E8" s="22"/>
       <c r="F8" s="23"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B9" s="16"/>
       <c r="C9" s="4"/>
       <c r="D9" s="21" t="s">
@@ -1215,7 +1207,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B10" s="16"/>
       <c r="C10" s="4"/>
       <c r="D10" s="21" t="s">
@@ -1224,7 +1216,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B11" s="17"/>
       <c r="C11" s="13"/>
       <c r="D11" s="24" t="s">
@@ -1233,7 +1225,7 @@
       <c r="E11" s="25"/>
       <c r="F11" s="26"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B12" s="15" t="s">
         <v>6</v>
       </c>
@@ -1244,7 +1236,7 @@
       <c r="E12" s="19"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B13" s="16"/>
       <c r="C13" s="12"/>
       <c r="D13" s="21" t="s">
@@ -1253,7 +1245,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="23"/>
     </row>
-    <row r="14" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="17"/>
       <c r="C14" s="13"/>
       <c r="D14" s="24" t="s">
@@ -1262,14 +1254,14 @@
       <c r="E14" s="25"/>
       <c r="F14" s="26"/>
     </row>
-    <row r="15" spans="2:6" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:6" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B16" s="27" t="s">
         <v>3</v>
       </c>
@@ -1282,7 +1274,7 @@
       </c>
       <c r="F16" s="14"/>
     </row>
-    <row r="17" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B17" s="29" t="s">
         <v>2</v>
       </c>
@@ -1297,7 +1289,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:22" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:22" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="31" t="s">
         <v>5</v>
       </c>
@@ -1306,7 +1298,7 @@
       <c r="E18" s="32"/>
       <c r="F18" s="33"/>
     </row>
-    <row r="19" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:22" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B19" s="34" t="s">
         <v>17</v>
       </c>
@@ -1317,7 +1309,7 @@
       <c r="E19" s="19"/>
       <c r="F19" s="20"/>
     </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B20" s="16"/>
       <c r="C20" s="4"/>
       <c r="D20" s="21" t="s">
@@ -1326,7 +1318,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="23"/>
     </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B21" s="16"/>
       <c r="C21" s="4"/>
       <c r="D21" s="21" t="s">
@@ -1335,7 +1327,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="23"/>
     </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B22" s="16"/>
       <c r="C22" s="4"/>
       <c r="D22" s="21" t="s">
@@ -1344,7 +1336,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="23"/>
     </row>
-    <row r="23" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B23" s="17"/>
       <c r="C23" s="13"/>
       <c r="D23" s="24" t="s">
@@ -1353,7 +1345,7 @@
       <c r="E23" s="25"/>
       <c r="F23" s="26"/>
     </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B24" s="15" t="s">
         <v>6</v>
       </c>
@@ -1364,7 +1356,7 @@
       <c r="E24" s="19"/>
       <c r="F24" s="20"/>
     </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B25" s="16"/>
       <c r="C25" s="12"/>
       <c r="D25" s="21" t="s">
@@ -1373,7 +1365,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="23"/>
     </row>
-    <row r="26" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" s="17"/>
       <c r="C26" s="13"/>
       <c r="D26" s="24" t="s">
@@ -1382,14 +1374,14 @@
       <c r="E26" s="25"/>
       <c r="F26" s="26"/>
     </row>
-    <row r="27" spans="2:22" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:22" s="7" customFormat="1" ht="6.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B28" s="27" t="s">
         <v>3</v>
       </c>
@@ -1402,7 +1394,7 @@
       </c>
       <c r="F28" s="14"/>
     </row>
-    <row r="29" spans="2:22" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B29" s="29" t="s">
         <v>2</v>
       </c>
@@ -1417,7 +1409,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:22" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:22" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B30" s="31" t="s">
         <v>5</v>
       </c>
@@ -1426,7 +1418,7 @@
       <c r="E30" s="32"/>
       <c r="F30" s="33"/>
     </row>
-    <row r="31" spans="2:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:22" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B31" s="34" t="s">
         <v>17</v>
       </c>
@@ -1437,7 +1429,7 @@
       <c r="E31" s="19"/>
       <c r="F31" s="20"/>
     </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:22" x14ac:dyDescent="0.4">
       <c r="B32" s="16"/>
       <c r="C32" s="4"/>
       <c r="D32" s="21" t="s">
@@ -1449,7 +1441,7 @@
         <v>44267</v>
       </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B33" s="16"/>
       <c r="C33" s="4"/>
       <c r="D33" s="21" t="s">
@@ -1458,7 +1450,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="23"/>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B34" s="16"/>
       <c r="C34" s="4"/>
       <c r="D34" s="21" t="s">
@@ -1467,7 +1459,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="23"/>
     </row>
-    <row r="35" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B35" s="17"/>
       <c r="C35" s="13"/>
       <c r="D35" s="24" t="s">
@@ -1476,7 +1468,7 @@
       <c r="E35" s="25"/>
       <c r="F35" s="26"/>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B36" s="15" t="s">
         <v>6</v>
       </c>
@@ -1487,7 +1479,7 @@
       <c r="E36" s="19"/>
       <c r="F36" s="20"/>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B37" s="16"/>
       <c r="C37" s="12"/>
       <c r="D37" s="21" t="s">
@@ -1496,7 +1488,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="23"/>
     </row>
-    <row r="38" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B38" s="17"/>
       <c r="C38" s="13"/>
       <c r="D38" s="24" t="s">
@@ -1505,8 +1497,8 @@
       <c r="E38" s="25"/>
       <c r="F38" s="26"/>
     </row>
-    <row r="39" spans="2:6" ht="7.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:6" ht="7.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B40" s="27" t="s">
         <v>3</v>
       </c>
@@ -1519,7 +1511,7 @@
       </c>
       <c r="F40" s="14"/>
     </row>
-    <row r="41" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B41" s="29" t="s">
         <v>2</v>
       </c>
@@ -1534,7 +1526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B42" s="31" t="s">
         <v>5</v>
       </c>
@@ -1543,7 +1535,7 @@
       <c r="E42" s="32"/>
       <c r="F42" s="33"/>
     </row>
-    <row r="43" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B43" s="34" t="s">
         <v>17</v>
       </c>
@@ -1554,7 +1546,7 @@
       <c r="E43" s="19"/>
       <c r="F43" s="20"/>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B44" s="16"/>
       <c r="C44" s="4"/>
       <c r="D44" s="21" t="s">
@@ -1563,7 +1555,7 @@
       <c r="E44" s="22"/>
       <c r="F44" s="23"/>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B45" s="16"/>
       <c r="C45" s="4"/>
       <c r="D45" s="21" t="s">
@@ -1572,7 +1564,7 @@
       <c r="E45" s="22"/>
       <c r="F45" s="23"/>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B46" s="16"/>
       <c r="C46" s="4"/>
       <c r="D46" s="21" t="s">
@@ -1581,7 +1573,7 @@
       <c r="E46" s="22"/>
       <c r="F46" s="23"/>
     </row>
-    <row r="47" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B47" s="17"/>
       <c r="C47" s="13"/>
       <c r="D47" s="24" t="s">
@@ -1590,7 +1582,7 @@
       <c r="E47" s="25"/>
       <c r="F47" s="26"/>
     </row>
-    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B48" s="15" t="s">
         <v>6</v>
       </c>
@@ -1601,7 +1593,7 @@
       <c r="E48" s="19"/>
       <c r="F48" s="20"/>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B49" s="16"/>
       <c r="C49" s="12"/>
       <c r="D49" s="21" t="s">
@@ -1610,7 +1602,7 @@
       <c r="E49" s="22"/>
       <c r="F49" s="23"/>
     </row>
-    <row r="50" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B50" s="17"/>
       <c r="C50" s="13"/>
       <c r="D50" s="24" t="s">
@@ -1619,8 +1611,8 @@
       <c r="E50" s="25"/>
       <c r="F50" s="26"/>
     </row>
-    <row r="51" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B52" s="27" t="s">
         <v>3</v>
       </c>
@@ -1633,7 +1625,7 @@
       </c>
       <c r="F52" s="14"/>
     </row>
-    <row r="53" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B53" s="29" t="s">
         <v>2</v>
       </c>
@@ -1648,7 +1640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B54" s="31" t="s">
         <v>5</v>
       </c>
@@ -1657,7 +1649,7 @@
       <c r="E54" s="32"/>
       <c r="F54" s="33"/>
     </row>
-    <row r="55" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B55" s="34" t="s">
         <v>17</v>
       </c>
@@ -1668,7 +1660,7 @@
       <c r="E55" s="19"/>
       <c r="F55" s="20"/>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B56" s="16"/>
       <c r="C56" s="4"/>
       <c r="D56" s="21" t="s">
@@ -1677,7 +1669,7 @@
       <c r="E56" s="22"/>
       <c r="F56" s="23"/>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B57" s="16"/>
       <c r="C57" s="4"/>
       <c r="D57" s="21" t="s">
@@ -1686,7 +1678,7 @@
       <c r="E57" s="22"/>
       <c r="F57" s="23"/>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B58" s="16"/>
       <c r="C58" s="4"/>
       <c r="D58" s="21" t="s">
@@ -1695,7 +1687,7 @@
       <c r="E58" s="22"/>
       <c r="F58" s="23"/>
     </row>
-    <row r="59" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B59" s="17"/>
       <c r="C59" s="13"/>
       <c r="D59" s="24" t="s">
@@ -1704,7 +1696,7 @@
       <c r="E59" s="25"/>
       <c r="F59" s="26"/>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B60" s="15" t="s">
         <v>6</v>
       </c>
@@ -1715,7 +1707,7 @@
       <c r="E60" s="19"/>
       <c r="F60" s="20"/>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B61" s="16"/>
       <c r="C61" s="12"/>
       <c r="D61" s="21" t="s">
@@ -1724,7 +1716,7 @@
       <c r="E61" s="22"/>
       <c r="F61" s="23"/>
     </row>
-    <row r="62" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B62" s="17"/>
       <c r="C62" s="13"/>
       <c r="D62" s="24" t="s">
@@ -1733,122 +1725,8 @@
       <c r="E62" s="25"/>
       <c r="F62" s="26"/>
     </row>
-    <row r="63" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B64" s="27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C64" s="28"/>
-      <c r="D64" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F64" s="14"/>
-    </row>
-    <row r="65" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B65" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="30"/>
-      <c r="D65" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B66" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="33"/>
-    </row>
-    <row r="67" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B67" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="19"/>
-      <c r="F67" s="20"/>
-    </row>
-    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B68" s="16"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E68" s="22"/>
-      <c r="F68" s="23"/>
-    </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B69" s="16"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E69" s="22"/>
-      <c r="F69" s="23"/>
-    </row>
-    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B70" s="16"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E70" s="22"/>
-      <c r="F70" s="23"/>
-    </row>
-    <row r="71" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B71" s="17"/>
-      <c r="C71" s="13"/>
-      <c r="D71" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="E71" s="25"/>
-      <c r="F71" s="26"/>
-    </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B72" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" s="1"/>
-      <c r="D72" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="E72" s="19"/>
-      <c r="F72" s="20"/>
-    </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B73" s="16"/>
-      <c r="C73" s="12"/>
-      <c r="D73" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E73" s="22"/>
-      <c r="F73" s="23"/>
-    </row>
-    <row r="74" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B74" s="17"/>
-      <c r="C74" s="13"/>
-      <c r="D74" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="E74" s="25"/>
-      <c r="F74" s="26"/>
-    </row>
-    <row r="75" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B76" s="27" t="s">
         <v>3</v>
       </c>
@@ -1861,7 +1739,7 @@
       </c>
       <c r="F76" s="14"/>
     </row>
-    <row r="77" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B77" s="29" t="s">
         <v>2</v>
       </c>
@@ -1876,7 +1754,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="78" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B78" s="31" t="s">
         <v>5</v>
       </c>
@@ -1885,7 +1763,7 @@
       <c r="E78" s="32"/>
       <c r="F78" s="33"/>
     </row>
-    <row r="79" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B79" s="34" t="s">
         <v>17</v>
       </c>
@@ -1896,7 +1774,7 @@
       <c r="E79" s="19"/>
       <c r="F79" s="20"/>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B80" s="16"/>
       <c r="C80" s="4"/>
       <c r="D80" s="21" t="s">
@@ -1905,7 +1783,7 @@
       <c r="E80" s="22"/>
       <c r="F80" s="23"/>
     </row>
-    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B81" s="16"/>
       <c r="C81" s="4"/>
       <c r="D81" s="21" t="s">
@@ -1914,7 +1792,7 @@
       <c r="E81" s="22"/>
       <c r="F81" s="23"/>
     </row>
-    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B82" s="16"/>
       <c r="C82" s="4"/>
       <c r="D82" s="21" t="s">
@@ -1923,7 +1801,7 @@
       <c r="E82" s="22"/>
       <c r="F82" s="23"/>
     </row>
-    <row r="83" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B83" s="17"/>
       <c r="C83" s="13"/>
       <c r="D83" s="24" t="s">
@@ -1932,7 +1810,7 @@
       <c r="E83" s="25"/>
       <c r="F83" s="26"/>
     </row>
-    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B84" s="15" t="s">
         <v>6</v>
       </c>
@@ -1943,7 +1821,7 @@
       <c r="E84" s="19"/>
       <c r="F84" s="20"/>
     </row>
-    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B85" s="16"/>
       <c r="C85" s="12"/>
       <c r="D85" s="21" t="s">
@@ -1952,7 +1830,7 @@
       <c r="E85" s="22"/>
       <c r="F85" s="23"/>
     </row>
-    <row r="86" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B86" s="17"/>
       <c r="C86" s="13"/>
       <c r="D86" s="24" t="s">
@@ -1961,8 +1839,8 @@
       <c r="E86" s="25"/>
       <c r="F86" s="26"/>
     </row>
-    <row r="87" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B88" s="27" t="s">
         <v>3</v>
       </c>
@@ -1975,7 +1853,7 @@
       </c>
       <c r="F88" s="14"/>
     </row>
-    <row r="89" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B89" s="29" t="s">
         <v>2</v>
       </c>
@@ -1990,7 +1868,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="90" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B90" s="31" t="s">
         <v>5</v>
       </c>
@@ -1999,7 +1877,7 @@
       <c r="E90" s="32"/>
       <c r="F90" s="33"/>
     </row>
-    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B91" s="34" t="s">
         <v>17</v>
       </c>
@@ -2010,7 +1888,7 @@
       <c r="E91" s="19"/>
       <c r="F91" s="20"/>
     </row>
-    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B92" s="16"/>
       <c r="C92" s="4"/>
       <c r="D92" s="21" t="s">
@@ -2019,7 +1897,7 @@
       <c r="E92" s="22"/>
       <c r="F92" s="23"/>
     </row>
-    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B93" s="16"/>
       <c r="C93" s="4"/>
       <c r="D93" s="21" t="s">
@@ -2028,7 +1906,7 @@
       <c r="E93" s="22"/>
       <c r="F93" s="23"/>
     </row>
-    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B94" s="16"/>
       <c r="C94" s="4"/>
       <c r="D94" s="21" t="s">
@@ -2037,7 +1915,7 @@
       <c r="E94" s="22"/>
       <c r="F94" s="23"/>
     </row>
-    <row r="95" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B95" s="17"/>
       <c r="C95" s="13"/>
       <c r="D95" s="24" t="s">
@@ -2046,7 +1924,7 @@
       <c r="E95" s="25"/>
       <c r="F95" s="26"/>
     </row>
-    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B96" s="15" t="s">
         <v>6</v>
       </c>
@@ -2057,7 +1935,7 @@
       <c r="E96" s="19"/>
       <c r="F96" s="20"/>
     </row>
-    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B97" s="16"/>
       <c r="C97" s="12"/>
       <c r="D97" s="21" t="s">
@@ -2066,7 +1944,7 @@
       <c r="E97" s="22"/>
       <c r="F97" s="23"/>
     </row>
-    <row r="98" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B98" s="17"/>
       <c r="C98" s="13"/>
       <c r="D98" s="24" t="s">
@@ -2075,8 +1953,8 @@
       <c r="E98" s="25"/>
       <c r="F98" s="26"/>
     </row>
-    <row r="99" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B100" s="27" t="s">
         <v>3</v>
       </c>
@@ -2089,7 +1967,7 @@
       </c>
       <c r="F100" s="14"/>
     </row>
-    <row r="101" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B101" s="29" t="s">
         <v>2</v>
       </c>
@@ -2104,7 +1982,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B102" s="31" t="s">
         <v>5</v>
       </c>
@@ -2113,7 +1991,7 @@
       <c r="E102" s="32"/>
       <c r="F102" s="33"/>
     </row>
-    <row r="103" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B103" s="34" t="s">
         <v>17</v>
       </c>
@@ -2124,7 +2002,7 @@
       <c r="E103" s="19"/>
       <c r="F103" s="20"/>
     </row>
-    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B104" s="16"/>
       <c r="C104" s="4"/>
       <c r="D104" s="21" t="s">
@@ -2133,7 +2011,7 @@
       <c r="E104" s="22"/>
       <c r="F104" s="23"/>
     </row>
-    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B105" s="16"/>
       <c r="C105" s="4"/>
       <c r="D105" s="21" t="s">
@@ -2142,7 +2020,7 @@
       <c r="E105" s="22"/>
       <c r="F105" s="23"/>
     </row>
-    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B106" s="16"/>
       <c r="C106" s="4"/>
       <c r="D106" s="21" t="s">
@@ -2151,7 +2029,7 @@
       <c r="E106" s="22"/>
       <c r="F106" s="23"/>
     </row>
-    <row r="107" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B107" s="17"/>
       <c r="C107" s="13"/>
       <c r="D107" s="24" t="s">
@@ -2160,7 +2038,7 @@
       <c r="E107" s="25"/>
       <c r="F107" s="26"/>
     </row>
-    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B108" s="15" t="s">
         <v>6</v>
       </c>
@@ -2171,7 +2049,7 @@
       <c r="E108" s="19"/>
       <c r="F108" s="20"/>
     </row>
-    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B109" s="16"/>
       <c r="C109" s="12"/>
       <c r="D109" s="21" t="s">
@@ -2180,7 +2058,7 @@
       <c r="E109" s="22"/>
       <c r="F109" s="23"/>
     </row>
-    <row r="110" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B110" s="17"/>
       <c r="C110" s="13"/>
       <c r="D110" s="24" t="s">
@@ -2189,8 +2067,8 @@
       <c r="E110" s="25"/>
       <c r="F110" s="26"/>
     </row>
-    <row r="111" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B112" s="27" t="s">
         <v>3</v>
       </c>
@@ -2203,7 +2081,7 @@
       </c>
       <c r="F112" s="14"/>
     </row>
-    <row r="113" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B113" s="29" t="s">
         <v>2</v>
       </c>
@@ -2218,7 +2096,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B114" s="31" t="s">
         <v>5</v>
       </c>
@@ -2227,7 +2105,7 @@
       <c r="E114" s="32"/>
       <c r="F114" s="33"/>
     </row>
-    <row r="115" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B115" s="34" t="s">
         <v>17</v>
       </c>
@@ -2238,8 +2116,8 @@
       <c r="E115" s="19"/>
       <c r="F115" s="20"/>
     </row>
-    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B116" s="35"/>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B116" s="36"/>
       <c r="C116" s="4"/>
       <c r="D116" s="21" t="s">
         <v>10</v>
@@ -2247,8 +2125,8 @@
       <c r="E116" s="22"/>
       <c r="F116" s="23"/>
     </row>
-    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B117" s="35"/>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B117" s="36"/>
       <c r="C117" s="4"/>
       <c r="D117" s="21" t="s">
         <v>11</v>
@@ -2256,8 +2134,8 @@
       <c r="E117" s="22"/>
       <c r="F117" s="23"/>
     </row>
-    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B118" s="35"/>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.4">
+      <c r="B118" s="36"/>
       <c r="C118" s="4"/>
       <c r="D118" s="21" t="s">
         <v>12</v>
@@ -2265,8 +2143,8 @@
       <c r="E118" s="22"/>
       <c r="F118" s="23"/>
     </row>
-    <row r="119" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B119" s="36"/>
+    <row r="119" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B119" s="37"/>
       <c r="C119" s="13"/>
       <c r="D119" s="24" t="s">
         <v>13</v>
@@ -2274,7 +2152,7 @@
       <c r="E119" s="25"/>
       <c r="F119" s="26"/>
     </row>
-    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B120" s="15" t="s">
         <v>6</v>
       </c>
@@ -2285,7 +2163,7 @@
       <c r="E120" s="19"/>
       <c r="F120" s="20"/>
     </row>
-    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B121" s="16"/>
       <c r="C121" s="12"/>
       <c r="D121" s="21" t="s">
@@ -2294,7 +2172,7 @@
       <c r="E121" s="22"/>
       <c r="F121" s="23"/>
     </row>
-    <row r="122" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B122" s="17"/>
       <c r="C122" s="13"/>
       <c r="D122" s="24" t="s">
@@ -2303,8 +2181,8 @@
       <c r="E122" s="25"/>
       <c r="F122" s="26"/>
     </row>
-    <row r="123" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B124" s="27" t="s">
         <v>3</v>
       </c>
@@ -2317,7 +2195,7 @@
       </c>
       <c r="F124" s="14"/>
     </row>
-    <row r="125" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B125" s="29" t="s">
         <v>2</v>
       </c>
@@ -2332,7 +2210,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="126" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B126" s="31" t="s">
         <v>5</v>
       </c>
@@ -2341,7 +2219,7 @@
       <c r="E126" s="32"/>
       <c r="F126" s="33"/>
     </row>
-    <row r="127" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B127" s="34" t="s">
         <v>17</v>
       </c>
@@ -2352,7 +2230,7 @@
       <c r="E127" s="19"/>
       <c r="F127" s="20"/>
     </row>
-    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B128" s="16"/>
       <c r="C128" s="4"/>
       <c r="D128" s="21" t="s">
@@ -2361,7 +2239,7 @@
       <c r="E128" s="22"/>
       <c r="F128" s="23"/>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B129" s="16"/>
       <c r="C129" s="4"/>
       <c r="D129" s="21" t="s">
@@ -2370,7 +2248,7 @@
       <c r="E129" s="22"/>
       <c r="F129" s="23"/>
     </row>
-    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B130" s="16"/>
       <c r="C130" s="4"/>
       <c r="D130" s="21" t="s">
@@ -2379,7 +2257,7 @@
       <c r="E130" s="22"/>
       <c r="F130" s="23"/>
     </row>
-    <row r="131" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B131" s="17"/>
       <c r="C131" s="13"/>
       <c r="D131" s="24" t="s">
@@ -2388,7 +2266,7 @@
       <c r="E131" s="25"/>
       <c r="F131" s="26"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B132" s="15" t="s">
         <v>6</v>
       </c>
@@ -2399,7 +2277,7 @@
       <c r="E132" s="19"/>
       <c r="F132" s="20"/>
     </row>
-    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B133" s="16"/>
       <c r="C133" s="12"/>
       <c r="D133" s="21" t="s">
@@ -2408,7 +2286,7 @@
       <c r="E133" s="22"/>
       <c r="F133" s="23"/>
     </row>
-    <row r="134" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B134" s="17"/>
       <c r="C134" s="13"/>
       <c r="D134" s="24" t="s">
@@ -2417,8 +2295,8 @@
       <c r="E134" s="25"/>
       <c r="F134" s="26"/>
     </row>
-    <row r="135" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B136" s="27" t="s">
         <v>3</v>
       </c>
@@ -2431,7 +2309,7 @@
       </c>
       <c r="F136" s="14"/>
     </row>
-    <row r="137" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B137" s="29" t="s">
         <v>2</v>
       </c>
@@ -2446,7 +2324,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="138" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B138" s="31" t="s">
         <v>5</v>
       </c>
@@ -2455,7 +2333,7 @@
       <c r="E138" s="32"/>
       <c r="F138" s="33"/>
     </row>
-    <row r="139" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B139" s="34" t="s">
         <v>17</v>
       </c>
@@ -2466,7 +2344,7 @@
       <c r="E139" s="19"/>
       <c r="F139" s="20"/>
     </row>
-    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B140" s="16"/>
       <c r="C140" s="4"/>
       <c r="D140" s="21" t="s">
@@ -2475,7 +2353,7 @@
       <c r="E140" s="22"/>
       <c r="F140" s="23"/>
     </row>
-    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B141" s="16"/>
       <c r="C141" s="4"/>
       <c r="D141" s="21" t="s">
@@ -2484,7 +2362,7 @@
       <c r="E141" s="22"/>
       <c r="F141" s="23"/>
     </row>
-    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B142" s="16"/>
       <c r="C142" s="4"/>
       <c r="D142" s="21" t="s">
@@ -2493,7 +2371,7 @@
       <c r="E142" s="22"/>
       <c r="F142" s="23"/>
     </row>
-    <row r="143" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B143" s="17"/>
       <c r="C143" s="13"/>
       <c r="D143" s="24" t="s">
@@ -2502,7 +2380,7 @@
       <c r="E143" s="25"/>
       <c r="F143" s="26"/>
     </row>
-    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B144" s="15" t="s">
         <v>6</v>
       </c>
@@ -2513,7 +2391,7 @@
       <c r="E144" s="19"/>
       <c r="F144" s="20"/>
     </row>
-    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B145" s="16"/>
       <c r="C145" s="12"/>
       <c r="D145" s="21" t="s">
@@ -2522,7 +2400,7 @@
       <c r="E145" s="22"/>
       <c r="F145" s="23"/>
     </row>
-    <row r="146" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B146" s="17"/>
       <c r="C146" s="13"/>
       <c r="D146" s="24" t="s">
@@ -2531,8 +2409,8 @@
       <c r="E146" s="25"/>
       <c r="F146" s="26"/>
     </row>
-    <row r="147" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="148" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="148" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B148" s="27" t="s">
         <v>3</v>
       </c>
@@ -2545,7 +2423,7 @@
       </c>
       <c r="F148" s="14"/>
     </row>
-    <row r="149" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B149" s="29" t="s">
         <v>2</v>
       </c>
@@ -2560,7 +2438,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="150" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B150" s="31" t="s">
         <v>5</v>
       </c>
@@ -2569,7 +2447,7 @@
       <c r="E150" s="32"/>
       <c r="F150" s="33"/>
     </row>
-    <row r="151" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B151" s="34" t="s">
         <v>17</v>
       </c>
@@ -2580,7 +2458,7 @@
       <c r="E151" s="19"/>
       <c r="F151" s="20"/>
     </row>
-    <row r="152" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B152" s="16"/>
       <c r="C152" s="4"/>
       <c r="D152" s="21" t="s">
@@ -2589,7 +2467,7 @@
       <c r="E152" s="22"/>
       <c r="F152" s="23"/>
     </row>
-    <row r="153" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B153" s="16"/>
       <c r="C153" s="4"/>
       <c r="D153" s="21" t="s">
@@ -2598,7 +2476,7 @@
       <c r="E153" s="22"/>
       <c r="F153" s="23"/>
     </row>
-    <row r="154" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B154" s="16"/>
       <c r="C154" s="4"/>
       <c r="D154" s="21" t="s">
@@ -2607,7 +2485,7 @@
       <c r="E154" s="22"/>
       <c r="F154" s="23"/>
     </row>
-    <row r="155" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B155" s="17"/>
       <c r="C155" s="13"/>
       <c r="D155" s="24" t="s">
@@ -2616,7 +2494,7 @@
       <c r="E155" s="25"/>
       <c r="F155" s="26"/>
     </row>
-    <row r="156" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B156" s="15" t="s">
         <v>6</v>
       </c>
@@ -2627,7 +2505,7 @@
       <c r="E156" s="19"/>
       <c r="F156" s="20"/>
     </row>
-    <row r="157" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B157" s="16"/>
       <c r="C157" s="12"/>
       <c r="D157" s="21" t="s">
@@ -2636,7 +2514,7 @@
       <c r="E157" s="22"/>
       <c r="F157" s="23"/>
     </row>
-    <row r="158" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B158" s="17"/>
       <c r="C158" s="13"/>
       <c r="D158" s="24" t="s">
@@ -2645,8 +2523,8 @@
       <c r="E158" s="25"/>
       <c r="F158" s="26"/>
     </row>
-    <row r="159" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="160" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="160" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B160" s="27" t="s">
         <v>3</v>
       </c>
@@ -2659,7 +2537,7 @@
       </c>
       <c r="F160" s="14"/>
     </row>
-    <row r="161" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B161" s="29" t="s">
         <v>2</v>
       </c>
@@ -2674,7 +2552,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="162" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B162" s="31" t="s">
         <v>5</v>
       </c>
@@ -2683,7 +2561,7 @@
       <c r="E162" s="32"/>
       <c r="F162" s="33"/>
     </row>
-    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B163" s="34" t="s">
         <v>17</v>
       </c>
@@ -2694,7 +2572,7 @@
       <c r="E163" s="19"/>
       <c r="F163" s="20"/>
     </row>
-    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B164" s="16"/>
       <c r="C164" s="4"/>
       <c r="D164" s="21" t="s">
@@ -2703,7 +2581,7 @@
       <c r="E164" s="22"/>
       <c r="F164" s="23"/>
     </row>
-    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B165" s="16"/>
       <c r="C165" s="4"/>
       <c r="D165" s="21" t="s">
@@ -2712,7 +2590,7 @@
       <c r="E165" s="22"/>
       <c r="F165" s="23"/>
     </row>
-    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B166" s="16"/>
       <c r="C166" s="4"/>
       <c r="D166" s="21" t="s">
@@ -2721,7 +2599,7 @@
       <c r="E166" s="22"/>
       <c r="F166" s="23"/>
     </row>
-    <row r="167" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B167" s="17"/>
       <c r="C167" s="13"/>
       <c r="D167" s="24" t="s">
@@ -2730,7 +2608,7 @@
       <c r="E167" s="25"/>
       <c r="F167" s="26"/>
     </row>
-    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B168" s="15" t="s">
         <v>6</v>
       </c>
@@ -2741,7 +2619,7 @@
       <c r="E168" s="19"/>
       <c r="F168" s="20"/>
     </row>
-    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B169" s="16"/>
       <c r="C169" s="12"/>
       <c r="D169" s="21" t="s">
@@ -2750,7 +2628,7 @@
       <c r="E169" s="22"/>
       <c r="F169" s="23"/>
     </row>
-    <row r="170" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B170" s="17"/>
       <c r="C170" s="13"/>
       <c r="D170" s="24" t="s">
@@ -2759,8 +2637,8 @@
       <c r="E170" s="25"/>
       <c r="F170" s="26"/>
     </row>
-    <row r="171" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B172" s="27" t="s">
         <v>3</v>
       </c>
@@ -2773,7 +2651,7 @@
       </c>
       <c r="F172" s="14"/>
     </row>
-    <row r="173" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B173" s="29" t="s">
         <v>2</v>
       </c>
@@ -2788,7 +2666,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="174" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B174" s="31" t="s">
         <v>5</v>
       </c>
@@ -2797,7 +2675,7 @@
       <c r="E174" s="32"/>
       <c r="F174" s="33"/>
     </row>
-    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B175" s="34" t="s">
         <v>17</v>
       </c>
@@ -2808,7 +2686,7 @@
       <c r="E175" s="19"/>
       <c r="F175" s="20"/>
     </row>
-    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B176" s="16"/>
       <c r="C176" s="4"/>
       <c r="D176" s="21" t="s">
@@ -2817,7 +2695,7 @@
       <c r="E176" s="22"/>
       <c r="F176" s="23"/>
     </row>
-    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B177" s="16"/>
       <c r="C177" s="4"/>
       <c r="D177" s="21" t="s">
@@ -2826,7 +2704,7 @@
       <c r="E177" s="22"/>
       <c r="F177" s="23"/>
     </row>
-    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B178" s="16"/>
       <c r="C178" s="4"/>
       <c r="D178" s="21" t="s">
@@ -2835,7 +2713,7 @@
       <c r="E178" s="22"/>
       <c r="F178" s="23"/>
     </row>
-    <row r="179" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B179" s="17"/>
       <c r="C179" s="13"/>
       <c r="D179" s="24" t="s">
@@ -2844,7 +2722,7 @@
       <c r="E179" s="25"/>
       <c r="F179" s="26"/>
     </row>
-    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B180" s="15" t="s">
         <v>6</v>
       </c>
@@ -2855,7 +2733,7 @@
       <c r="E180" s="19"/>
       <c r="F180" s="20"/>
     </row>
-    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B181" s="16"/>
       <c r="C181" s="12"/>
       <c r="D181" s="21" t="s">
@@ -2864,7 +2742,7 @@
       <c r="E181" s="22"/>
       <c r="F181" s="23"/>
     </row>
-    <row r="182" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B182" s="17"/>
       <c r="C182" s="13"/>
       <c r="D182" s="24" t="s">
@@ -2873,8 +2751,8 @@
       <c r="E182" s="25"/>
       <c r="F182" s="26"/>
     </row>
-    <row r="183" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B184" s="27" t="s">
         <v>3</v>
       </c>
@@ -2887,7 +2765,7 @@
       </c>
       <c r="F184" s="14"/>
     </row>
-    <row r="185" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B185" s="29" t="s">
         <v>2</v>
       </c>
@@ -2902,7 +2780,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="186" spans="2:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="2:6" ht="25.8" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B186" s="31" t="s">
         <v>5</v>
       </c>
@@ -2911,7 +2789,7 @@
       <c r="E186" s="32"/>
       <c r="F186" s="33"/>
     </row>
-    <row r="187" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B187" s="34" t="s">
         <v>17</v>
       </c>
@@ -2922,7 +2800,7 @@
       <c r="E187" s="19"/>
       <c r="F187" s="20"/>
     </row>
-    <row r="188" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B188" s="16"/>
       <c r="C188" s="4"/>
       <c r="D188" s="21" t="s">
@@ -2931,7 +2809,7 @@
       <c r="E188" s="22"/>
       <c r="F188" s="23"/>
     </row>
-    <row r="189" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B189" s="16"/>
       <c r="C189" s="4"/>
       <c r="D189" s="21" t="s">
@@ -2940,7 +2818,7 @@
       <c r="E189" s="22"/>
       <c r="F189" s="23"/>
     </row>
-    <row r="190" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B190" s="16"/>
       <c r="C190" s="4"/>
       <c r="D190" s="21" t="s">
@@ -2949,7 +2827,7 @@
       <c r="E190" s="22"/>
       <c r="F190" s="23"/>
     </row>
-    <row r="191" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B191" s="17"/>
       <c r="C191" s="13"/>
       <c r="D191" s="24" t="s">
@@ -2958,7 +2836,7 @@
       <c r="E191" s="25"/>
       <c r="F191" s="26"/>
     </row>
-    <row r="192" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B192" s="15" t="s">
         <v>6</v>
       </c>
@@ -2969,7 +2847,7 @@
       <c r="E192" s="19"/>
       <c r="F192" s="20"/>
     </row>
-    <row r="193" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:6" x14ac:dyDescent="0.4">
       <c r="B193" s="16"/>
       <c r="C193" s="12"/>
       <c r="D193" s="21" t="s">
@@ -2978,7 +2856,7 @@
       <c r="E193" s="22"/>
       <c r="F193" s="23"/>
     </row>
-    <row r="194" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B194" s="17"/>
       <c r="C194" s="13"/>
       <c r="D194" s="24" t="s">
@@ -2988,20 +2866,179 @@
       <c r="F194" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="209">
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="D72:F72"/>
-    <mergeCell ref="D73:F73"/>
-    <mergeCell ref="D74:F74"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="B66:F66"/>
-    <mergeCell ref="B67:B71"/>
-    <mergeCell ref="D67:F67"/>
-    <mergeCell ref="D68:F68"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D70:F70"/>
-    <mergeCell ref="D71:F71"/>
+  <mergeCells count="196">
+    <mergeCell ref="B192:B194"/>
+    <mergeCell ref="D192:F192"/>
+    <mergeCell ref="D193:F193"/>
+    <mergeCell ref="D194:F194"/>
+    <mergeCell ref="B180:B182"/>
+    <mergeCell ref="D180:F180"/>
+    <mergeCell ref="D181:F181"/>
+    <mergeCell ref="D182:F182"/>
+    <mergeCell ref="B184:C184"/>
+    <mergeCell ref="B185:C185"/>
+    <mergeCell ref="B186:F186"/>
+    <mergeCell ref="B187:B191"/>
+    <mergeCell ref="D187:F187"/>
+    <mergeCell ref="D188:F188"/>
+    <mergeCell ref="D189:F189"/>
+    <mergeCell ref="D190:F190"/>
+    <mergeCell ref="D191:F191"/>
+    <mergeCell ref="B168:B170"/>
+    <mergeCell ref="D168:F168"/>
+    <mergeCell ref="D169:F169"/>
+    <mergeCell ref="D170:F170"/>
+    <mergeCell ref="B156:B158"/>
+    <mergeCell ref="D156:F156"/>
+    <mergeCell ref="D157:F157"/>
+    <mergeCell ref="D158:F158"/>
+    <mergeCell ref="B160:C160"/>
+    <mergeCell ref="B161:C161"/>
+    <mergeCell ref="B162:F162"/>
+    <mergeCell ref="B172:C172"/>
+    <mergeCell ref="B173:C173"/>
+    <mergeCell ref="B174:F174"/>
+    <mergeCell ref="B175:B179"/>
+    <mergeCell ref="D175:F175"/>
+    <mergeCell ref="D176:F176"/>
+    <mergeCell ref="D177:F177"/>
+    <mergeCell ref="D178:F178"/>
+    <mergeCell ref="D179:F179"/>
+    <mergeCell ref="B163:B167"/>
+    <mergeCell ref="D163:F163"/>
+    <mergeCell ref="D164:F164"/>
+    <mergeCell ref="D165:F165"/>
+    <mergeCell ref="D166:F166"/>
+    <mergeCell ref="D167:F167"/>
+    <mergeCell ref="B148:C148"/>
+    <mergeCell ref="B149:C149"/>
+    <mergeCell ref="B150:F150"/>
+    <mergeCell ref="B151:B155"/>
+    <mergeCell ref="D151:F151"/>
+    <mergeCell ref="D152:F152"/>
+    <mergeCell ref="D153:F153"/>
+    <mergeCell ref="D154:F154"/>
+    <mergeCell ref="D155:F155"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="D61:F61"/>
+    <mergeCell ref="D60:F60"/>
+    <mergeCell ref="D59:F59"/>
+    <mergeCell ref="D58:F58"/>
+    <mergeCell ref="D83:F83"/>
+    <mergeCell ref="D82:F82"/>
+    <mergeCell ref="D81:F81"/>
+    <mergeCell ref="D80:F80"/>
+    <mergeCell ref="D79:F79"/>
+    <mergeCell ref="D120:F120"/>
+    <mergeCell ref="D119:F119"/>
+    <mergeCell ref="D104:F104"/>
+    <mergeCell ref="D103:F103"/>
+    <mergeCell ref="D86:F86"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D84:F84"/>
+    <mergeCell ref="D109:F109"/>
+    <mergeCell ref="D108:F108"/>
+    <mergeCell ref="D107:F107"/>
+    <mergeCell ref="D106:F106"/>
+    <mergeCell ref="D105:F105"/>
+    <mergeCell ref="B90:F90"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="D91:F91"/>
+    <mergeCell ref="D92:F92"/>
+    <mergeCell ref="D93:F93"/>
+    <mergeCell ref="D94:F94"/>
+    <mergeCell ref="D95:F95"/>
+    <mergeCell ref="B96:B98"/>
+    <mergeCell ref="D96:F96"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="D98:F98"/>
+    <mergeCell ref="D146:F146"/>
+    <mergeCell ref="D145:F145"/>
+    <mergeCell ref="D144:F144"/>
+    <mergeCell ref="D143:F143"/>
+    <mergeCell ref="D142:F142"/>
+    <mergeCell ref="B144:B146"/>
+    <mergeCell ref="B137:C137"/>
+    <mergeCell ref="B138:F138"/>
+    <mergeCell ref="B139:B143"/>
+    <mergeCell ref="D141:F141"/>
+    <mergeCell ref="D140:F140"/>
+    <mergeCell ref="D139:F139"/>
+    <mergeCell ref="B132:B134"/>
+    <mergeCell ref="B136:C136"/>
+    <mergeCell ref="B125:C125"/>
+    <mergeCell ref="B126:F126"/>
+    <mergeCell ref="B127:B131"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="B113:C113"/>
+    <mergeCell ref="B114:F114"/>
+    <mergeCell ref="B115:B119"/>
+    <mergeCell ref="D132:F132"/>
+    <mergeCell ref="D131:F131"/>
+    <mergeCell ref="D130:F130"/>
+    <mergeCell ref="D129:F129"/>
+    <mergeCell ref="D128:F128"/>
+    <mergeCell ref="D134:F134"/>
+    <mergeCell ref="D133:F133"/>
+    <mergeCell ref="D118:F118"/>
+    <mergeCell ref="D117:F117"/>
+    <mergeCell ref="D116:F116"/>
+    <mergeCell ref="D115:F115"/>
+    <mergeCell ref="D127:F127"/>
+    <mergeCell ref="D122:F122"/>
+    <mergeCell ref="D121:F121"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B101:C101"/>
+    <mergeCell ref="B102:F102"/>
+    <mergeCell ref="B103:B107"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B78:F78"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="D110:F110"/>
+    <mergeCell ref="B88:C88"/>
+    <mergeCell ref="B89:C89"/>
+    <mergeCell ref="B60:B62"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D38:F38"/>
+    <mergeCell ref="D37:F37"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:F42"/>
+    <mergeCell ref="B43:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="D50:F50"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="D46:F46"/>
+    <mergeCell ref="D47:F47"/>
+    <mergeCell ref="D57:F57"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D55:F55"/>
     <mergeCell ref="D48:F48"/>
     <mergeCell ref="D44:F44"/>
     <mergeCell ref="D43:F43"/>
@@ -3026,178 +3063,6 @@
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:B11"/>
     <mergeCell ref="D7:F7"/>
-    <mergeCell ref="B60:B62"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B31:B35"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="D38:F38"/>
-    <mergeCell ref="D37:F37"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D49:F49"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:F42"/>
-    <mergeCell ref="B43:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="D50:F50"/>
-    <mergeCell ref="D45:F45"/>
-    <mergeCell ref="D46:F46"/>
-    <mergeCell ref="D47:F47"/>
-    <mergeCell ref="D57:F57"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D55:F55"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B101:C101"/>
-    <mergeCell ref="B102:F102"/>
-    <mergeCell ref="B103:B107"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B78:F78"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="D110:F110"/>
-    <mergeCell ref="B132:B134"/>
-    <mergeCell ref="B136:C136"/>
-    <mergeCell ref="B125:C125"/>
-    <mergeCell ref="B126:F126"/>
-    <mergeCell ref="B127:B131"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="B114:F114"/>
-    <mergeCell ref="B115:B119"/>
-    <mergeCell ref="D132:F132"/>
-    <mergeCell ref="D131:F131"/>
-    <mergeCell ref="D130:F130"/>
-    <mergeCell ref="D129:F129"/>
-    <mergeCell ref="D128:F128"/>
-    <mergeCell ref="D134:F134"/>
-    <mergeCell ref="D133:F133"/>
-    <mergeCell ref="D118:F118"/>
-    <mergeCell ref="D117:F117"/>
-    <mergeCell ref="D116:F116"/>
-    <mergeCell ref="D115:F115"/>
-    <mergeCell ref="D127:F127"/>
-    <mergeCell ref="D122:F122"/>
-    <mergeCell ref="D121:F121"/>
-    <mergeCell ref="D146:F146"/>
-    <mergeCell ref="D145:F145"/>
-    <mergeCell ref="D144:F144"/>
-    <mergeCell ref="D143:F143"/>
-    <mergeCell ref="D142:F142"/>
-    <mergeCell ref="B144:B146"/>
-    <mergeCell ref="B137:C137"/>
-    <mergeCell ref="B138:F138"/>
-    <mergeCell ref="B139:B143"/>
-    <mergeCell ref="D141:F141"/>
-    <mergeCell ref="D140:F140"/>
-    <mergeCell ref="D139:F139"/>
-    <mergeCell ref="D120:F120"/>
-    <mergeCell ref="D119:F119"/>
-    <mergeCell ref="D104:F104"/>
-    <mergeCell ref="D103:F103"/>
-    <mergeCell ref="D86:F86"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D84:F84"/>
-    <mergeCell ref="D109:F109"/>
-    <mergeCell ref="D108:F108"/>
-    <mergeCell ref="D107:F107"/>
-    <mergeCell ref="D106:F106"/>
-    <mergeCell ref="D105:F105"/>
-    <mergeCell ref="D62:F62"/>
-    <mergeCell ref="D61:F61"/>
-    <mergeCell ref="D60:F60"/>
-    <mergeCell ref="D59:F59"/>
-    <mergeCell ref="D58:F58"/>
-    <mergeCell ref="D83:F83"/>
-    <mergeCell ref="D82:F82"/>
-    <mergeCell ref="D81:F81"/>
-    <mergeCell ref="D80:F80"/>
-    <mergeCell ref="D79:F79"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="B12:B14"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="D21:F21"/>
-    <mergeCell ref="D22:F22"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="B163:B167"/>
-    <mergeCell ref="D163:F163"/>
-    <mergeCell ref="D164:F164"/>
-    <mergeCell ref="D165:F165"/>
-    <mergeCell ref="D166:F166"/>
-    <mergeCell ref="D167:F167"/>
-    <mergeCell ref="B148:C148"/>
-    <mergeCell ref="B149:C149"/>
-    <mergeCell ref="B150:F150"/>
-    <mergeCell ref="B151:B155"/>
-    <mergeCell ref="D151:F151"/>
-    <mergeCell ref="D152:F152"/>
-    <mergeCell ref="D153:F153"/>
-    <mergeCell ref="D154:F154"/>
-    <mergeCell ref="D155:F155"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="B89:C89"/>
-    <mergeCell ref="B90:F90"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="D91:F91"/>
-    <mergeCell ref="D92:F92"/>
-    <mergeCell ref="D93:F93"/>
-    <mergeCell ref="D94:F94"/>
-    <mergeCell ref="D95:F95"/>
-    <mergeCell ref="B96:B98"/>
-    <mergeCell ref="D96:F96"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="D98:F98"/>
-    <mergeCell ref="B172:C172"/>
-    <mergeCell ref="B173:C173"/>
-    <mergeCell ref="B174:F174"/>
-    <mergeCell ref="B175:B179"/>
-    <mergeCell ref="D175:F175"/>
-    <mergeCell ref="D176:F176"/>
-    <mergeCell ref="D177:F177"/>
-    <mergeCell ref="D178:F178"/>
-    <mergeCell ref="D179:F179"/>
-    <mergeCell ref="B168:B170"/>
-    <mergeCell ref="D168:F168"/>
-    <mergeCell ref="D169:F169"/>
-    <mergeCell ref="D170:F170"/>
-    <mergeCell ref="B156:B158"/>
-    <mergeCell ref="D156:F156"/>
-    <mergeCell ref="D157:F157"/>
-    <mergeCell ref="D158:F158"/>
-    <mergeCell ref="B160:C160"/>
-    <mergeCell ref="B161:C161"/>
-    <mergeCell ref="B162:F162"/>
-    <mergeCell ref="B192:B194"/>
-    <mergeCell ref="D192:F192"/>
-    <mergeCell ref="D193:F193"/>
-    <mergeCell ref="D194:F194"/>
-    <mergeCell ref="B180:B182"/>
-    <mergeCell ref="D180:F180"/>
-    <mergeCell ref="D181:F181"/>
-    <mergeCell ref="D182:F182"/>
-    <mergeCell ref="B184:C184"/>
-    <mergeCell ref="B185:C185"/>
-    <mergeCell ref="B186:F186"/>
-    <mergeCell ref="B187:B191"/>
-    <mergeCell ref="D187:F187"/>
-    <mergeCell ref="D188:F188"/>
-    <mergeCell ref="D189:F189"/>
-    <mergeCell ref="D190:F190"/>
-    <mergeCell ref="D191:F191"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
@@ -3216,9 +3081,8 @@
     <hyperlink ref="D89" r:id="rId13" xr:uid="{7C40CEFE-159E-4FC6-924D-B37EC16356EA}"/>
     <hyperlink ref="D173" r:id="rId14" xr:uid="{3C4884CC-3DD6-489C-A10B-4979429BFB14}"/>
     <hyperlink ref="D185" r:id="rId15" xr:uid="{0E3E8996-96B6-4733-8C92-A66BBD25E5A2}"/>
-    <hyperlink ref="D65" r:id="rId16" xr:uid="{BEC34909-D6A2-4408-B067-74B36A5BF584}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>